<commit_message>
added components for mechanical assembly to BOM
</commit_message>
<xml_diff>
--- a/Production Files/Rev_B/BOM_Solaranlage_Rev.B.xlsx
+++ b/Production Files/Rev_B/BOM_Solaranlage_Rev.B.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="150">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -443,6 +443,36 @@
   </si>
   <si>
     <t xml:space="preserve">Two pin crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuts M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZK M3X6-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200-pack of M3 screws for mechanical assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance bolt M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VT DA 12MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance bolts for mechanical assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screw M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK-E M3-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100-pack of M3 nuts for mechanical assembly</t>
   </si>
 </sst>
 </file>
@@ -527,7 +557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -550,6 +580,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -580,7 +614,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1392,8 +1426,68 @@
         <v>139</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F52" s="6"/>
+      <c r="F52" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F38">

</xml_diff>